<commit_message>
Updated test report of AMT_V3
Functionality test is added.
</commit_message>
<xml_diff>
--- a/AMT HALL EFFECT/07_TestReport/Rev 3/LMAT_AMT_V3_Test_Report.xlsx
+++ b/AMT HALL EFFECT/07_TestReport/Rev 3/LMAT_AMT_V3_Test_Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="669" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="669" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover page" sheetId="5" r:id="rId1"/>
@@ -2278,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -3371,8 +3371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3661,10 +3661,18 @@
       <c r="B19" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
+      <c r="C19" s="62">
+        <v>3.5169999999999999</v>
+      </c>
+      <c r="D19" s="62">
+        <v>1.992</v>
+      </c>
+      <c r="E19" s="62">
+        <v>1.992</v>
+      </c>
+      <c r="F19" s="62">
+        <v>3.512</v>
+      </c>
       <c r="G19" s="115" t="s">
         <v>114</v>
       </c>
@@ -3677,10 +3685,18 @@
       <c r="B20" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
+      <c r="C20" s="62">
+        <v>3.516</v>
+      </c>
+      <c r="D20" s="62">
+        <v>3.5150000000000001</v>
+      </c>
+      <c r="E20" s="62">
+        <v>1.9910000000000001</v>
+      </c>
+      <c r="F20" s="62">
+        <v>1.992</v>
+      </c>
       <c r="G20" s="115"/>
       <c r="H20" s="62" t="s">
         <v>113</v>
@@ -3691,10 +3707,18 @@
       <c r="B21" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
+      <c r="C21" s="62">
+        <v>1.998</v>
+      </c>
+      <c r="D21" s="62">
+        <v>3.5150000000000001</v>
+      </c>
+      <c r="E21" s="62">
+        <v>3.5110000000000001</v>
+      </c>
+      <c r="F21" s="62">
+        <v>1.992</v>
+      </c>
       <c r="G21" s="115"/>
       <c r="H21" s="62" t="s">
         <v>113</v>
@@ -3705,10 +3729,18 @@
       <c r="B22" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
+      <c r="C22" s="62">
+        <v>1.9970000000000001</v>
+      </c>
+      <c r="D22" s="62">
+        <v>1.992</v>
+      </c>
+      <c r="E22" s="62">
+        <v>3.5110000000000001</v>
+      </c>
+      <c r="F22" s="62">
+        <v>3.5110000000000001</v>
+      </c>
       <c r="G22" s="115"/>
       <c r="H22" s="62" t="s">
         <v>113</v>
@@ -3719,10 +3751,18 @@
       <c r="B23" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
+      <c r="C23" s="62">
+        <v>3.516</v>
+      </c>
+      <c r="D23" s="62">
+        <v>3.5139999999999998</v>
+      </c>
+      <c r="E23" s="62">
+        <v>3.512</v>
+      </c>
+      <c r="F23" s="62">
+        <v>3.512</v>
+      </c>
       <c r="G23" s="115"/>
       <c r="H23" s="62" t="s">
         <v>113</v>
@@ -3733,10 +3773,18 @@
       <c r="B24" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
+      <c r="C24" s="62">
+        <v>1.9970000000000001</v>
+      </c>
+      <c r="D24" s="62">
+        <v>3.516</v>
+      </c>
+      <c r="E24" s="62">
+        <v>1.9910000000000001</v>
+      </c>
+      <c r="F24" s="62">
+        <v>3.512</v>
+      </c>
       <c r="G24" s="115"/>
       <c r="H24" s="62" t="s">
         <v>113</v>
@@ -3759,10 +3807,18 @@
       <c r="B26" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
+      <c r="C26" s="62">
+        <v>3.492</v>
+      </c>
+      <c r="D26" s="62">
+        <v>1.986</v>
+      </c>
+      <c r="E26" s="62">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="F26" s="62">
+        <v>3.4910000000000001</v>
+      </c>
       <c r="G26" s="115" t="s">
         <v>114</v>
       </c>
@@ -3775,10 +3831,18 @@
       <c r="B27" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
+      <c r="C27" s="62">
+        <v>3.4929999999999999</v>
+      </c>
+      <c r="D27" s="62">
+        <v>3.49</v>
+      </c>
+      <c r="E27" s="62">
+        <v>1.996</v>
+      </c>
+      <c r="F27" s="62">
+        <v>1.9890000000000001</v>
+      </c>
       <c r="G27" s="115"/>
       <c r="H27" s="62" t="s">
         <v>113</v>
@@ -3789,10 +3853,18 @@
       <c r="B28" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
+      <c r="C28" s="62">
+        <v>1.99</v>
+      </c>
+      <c r="D28" s="62">
+        <v>3.4910000000000001</v>
+      </c>
+      <c r="E28" s="62">
+        <v>3.496</v>
+      </c>
+      <c r="F28" s="62">
+        <v>1.99</v>
+      </c>
       <c r="G28" s="115"/>
       <c r="H28" s="62" t="s">
         <v>113</v>
@@ -3803,10 +3875,18 @@
       <c r="B29" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
+      <c r="C29" s="62">
+        <v>1.99</v>
+      </c>
+      <c r="D29" s="62">
+        <v>1.986</v>
+      </c>
+      <c r="E29" s="62">
+        <v>3.4969999999999999</v>
+      </c>
+      <c r="F29" s="62">
+        <v>3.4940000000000002</v>
+      </c>
       <c r="G29" s="115"/>
       <c r="H29" s="62" t="s">
         <v>113</v>
@@ -3817,10 +3897,18 @@
       <c r="B30" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
+      <c r="C30" s="62">
+        <v>3.4929999999999999</v>
+      </c>
+      <c r="D30" s="62">
+        <v>3.4910000000000001</v>
+      </c>
+      <c r="E30" s="62">
+        <v>3.4969999999999999</v>
+      </c>
+      <c r="F30" s="62">
+        <v>3.4929999999999999</v>
+      </c>
       <c r="G30" s="115"/>
       <c r="H30" s="62" t="s">
         <v>113</v>
@@ -3831,10 +3919,18 @@
       <c r="B31" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
+      <c r="C31" s="62">
+        <v>1.9910000000000001</v>
+      </c>
+      <c r="D31" s="62">
+        <v>3.4929999999999999</v>
+      </c>
+      <c r="E31" s="62">
+        <v>1.996</v>
+      </c>
+      <c r="F31" s="62">
+        <v>3.4950000000000001</v>
+      </c>
       <c r="G31" s="115"/>
       <c r="H31" s="62" t="s">
         <v>113</v>
@@ -3857,10 +3953,18 @@
       <c r="B33" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
+      <c r="C33" s="62">
+        <v>3.5089999999999999</v>
+      </c>
+      <c r="D33" s="62">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="E33" s="62">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="F33" s="62">
+        <v>3.512</v>
+      </c>
       <c r="G33" s="115" t="s">
         <v>114</v>
       </c>
@@ -3873,10 +3977,18 @@
       <c r="B34" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
+      <c r="C34" s="62">
+        <v>3.508</v>
+      </c>
+      <c r="D34" s="62">
+        <v>3.5059999999999998</v>
+      </c>
+      <c r="E34" s="62">
+        <v>1.998</v>
+      </c>
+      <c r="F34" s="62">
+        <v>1.9970000000000001</v>
+      </c>
       <c r="G34" s="115"/>
       <c r="H34" s="62" t="s">
         <v>113</v>
@@ -3887,10 +3999,18 @@
       <c r="B35" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
+      <c r="C35" s="62">
+        <v>1.996</v>
+      </c>
+      <c r="D35" s="62">
+        <v>3.5049999999999999</v>
+      </c>
+      <c r="E35" s="62">
+        <v>3.51</v>
+      </c>
+      <c r="F35" s="62">
+        <v>1.998</v>
+      </c>
       <c r="G35" s="115"/>
       <c r="H35" s="62" t="s">
         <v>113</v>
@@ -3901,10 +4021,18 @@
       <c r="B36" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
+      <c r="C36" s="62">
+        <v>1.996</v>
+      </c>
+      <c r="D36" s="62">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="E36" s="62">
+        <v>3.51</v>
+      </c>
+      <c r="F36" s="62">
+        <v>3.5110000000000001</v>
+      </c>
       <c r="G36" s="115"/>
       <c r="H36" s="62" t="s">
         <v>113</v>
@@ -3915,10 +4043,18 @@
       <c r="B37" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="C37" s="62">
+        <v>3.5089999999999999</v>
+      </c>
+      <c r="D37" s="62">
+        <v>3.5059999999999998</v>
+      </c>
+      <c r="E37" s="62">
+        <v>3.51</v>
+      </c>
+      <c r="F37" s="62">
+        <v>3.512</v>
+      </c>
       <c r="G37" s="115"/>
       <c r="H37" s="62" t="s">
         <v>113</v>
@@ -3929,10 +4065,18 @@
       <c r="B38" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
+      <c r="C38" s="62">
+        <v>1.996</v>
+      </c>
+      <c r="D38" s="62">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="E38" s="62">
+        <v>2</v>
+      </c>
+      <c r="F38" s="62">
+        <v>3.5139999999999998</v>
+      </c>
       <c r="G38" s="115"/>
       <c r="H38" s="62" t="s">
         <v>113</v>
@@ -3955,10 +4099,18 @@
       <c r="B40" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="C40" s="6">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.99</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1.998</v>
+      </c>
+      <c r="F40" s="6">
+        <v>3.508</v>
+      </c>
       <c r="G40" s="115" t="s">
         <v>114</v>
       </c>
@@ -3971,10 +4123,18 @@
       <c r="B41" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="C41" s="6">
+        <v>3.508</v>
+      </c>
+      <c r="D41" s="6">
+        <v>3.5059999999999998</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1.9990000000000001</v>
+      </c>
+      <c r="F41" s="6">
+        <v>1.9930000000000001</v>
+      </c>
       <c r="G41" s="115"/>
       <c r="H41" s="59" t="s">
         <v>113</v>
@@ -3985,10 +4145,18 @@
       <c r="B42" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+      <c r="C42" s="6">
+        <v>1.992</v>
+      </c>
+      <c r="D42" s="6">
+        <v>3.5049999999999999</v>
+      </c>
+      <c r="E42" s="6">
+        <v>3.508</v>
+      </c>
+      <c r="F42" s="6">
+        <v>1.9930000000000001</v>
+      </c>
       <c r="G42" s="115"/>
       <c r="H42" s="59" t="s">
         <v>113</v>
@@ -3999,10 +4167,18 @@
       <c r="B43" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
+      <c r="C43" s="6">
+        <v>1.992</v>
+      </c>
+      <c r="D43" s="6">
+        <v>1.99</v>
+      </c>
+      <c r="E43" s="6">
+        <v>3.5110000000000001</v>
+      </c>
+      <c r="F43" s="6">
+        <v>3.51</v>
+      </c>
       <c r="G43" s="115"/>
       <c r="H43" s="59" t="s">
         <v>113</v>
@@ -4013,10 +4189,18 @@
       <c r="B44" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+      <c r="C44" s="6">
+        <v>3.508</v>
+      </c>
+      <c r="D44" s="6">
+        <v>3.5059999999999998</v>
+      </c>
+      <c r="E44" s="6">
+        <v>3.51</v>
+      </c>
+      <c r="F44" s="6">
+        <v>3.5110000000000001</v>
+      </c>
       <c r="G44" s="115"/>
       <c r="H44" s="59" t="s">
         <v>113</v>
@@ -4027,10 +4211,18 @@
       <c r="B45" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="C45" s="6">
+        <v>1.992</v>
+      </c>
+      <c r="D45" s="6">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="E45" s="6">
+        <v>2</v>
+      </c>
+      <c r="F45" s="6">
+        <v>3.512</v>
+      </c>
       <c r="G45" s="115"/>
       <c r="H45" s="59" t="s">
         <v>113</v>
@@ -4043,10 +4235,18 @@
       <c r="B47" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
+      <c r="C47" s="59">
+        <v>3.4980000000000002</v>
+      </c>
+      <c r="D47" s="59">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="E47" s="59">
+        <v>1.996</v>
+      </c>
+      <c r="F47" s="59">
+        <v>3.5059999999999998</v>
+      </c>
       <c r="G47" s="115" t="s">
         <v>114</v>
       </c>
@@ -4059,10 +4259,18 @@
       <c r="B48" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
+      <c r="C48" s="59">
+        <v>3.4990000000000001</v>
+      </c>
+      <c r="D48" s="59">
+        <v>3.5019999999999998</v>
+      </c>
+      <c r="E48" s="59">
+        <v>1.996</v>
+      </c>
+      <c r="F48" s="59">
+        <v>1.996</v>
+      </c>
       <c r="G48" s="115"/>
       <c r="H48" s="59" t="s">
         <v>113</v>
@@ -4073,10 +4281,18 @@
       <c r="B49" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
+      <c r="C49" s="59">
+        <v>1.994</v>
+      </c>
+      <c r="D49" s="59">
+        <v>3.5009999999999999</v>
+      </c>
+      <c r="E49" s="59">
+        <v>3.5049999999999999</v>
+      </c>
+      <c r="F49" s="59">
+        <v>1.9950000000000001</v>
+      </c>
       <c r="G49" s="115"/>
       <c r="H49" s="59" t="s">
         <v>113</v>
@@ -4087,10 +4303,18 @@
       <c r="B50" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
+      <c r="C50" s="59">
+        <v>1.9930000000000001</v>
+      </c>
+      <c r="D50" s="59">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="E50" s="59">
+        <v>3.504</v>
+      </c>
+      <c r="F50" s="59">
+        <v>3.5070000000000001</v>
+      </c>
       <c r="G50" s="115"/>
       <c r="H50" s="59" t="s">
         <v>113</v>
@@ -4101,10 +4325,18 @@
       <c r="B51" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
+      <c r="C51" s="59">
+        <v>3.4969999999999999</v>
+      </c>
+      <c r="D51" s="59">
+        <v>3.5009999999999999</v>
+      </c>
+      <c r="E51" s="59">
+        <v>3.5030000000000001</v>
+      </c>
+      <c r="F51" s="59">
+        <v>3.5059999999999998</v>
+      </c>
       <c r="G51" s="115"/>
       <c r="H51" s="59" t="s">
         <v>113</v>
@@ -4115,10 +4347,18 @@
       <c r="B52" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
+      <c r="C52" s="59">
+        <v>1.994</v>
+      </c>
+      <c r="D52" s="59">
+        <v>3.5019999999999998</v>
+      </c>
+      <c r="E52" s="59">
+        <v>1.996</v>
+      </c>
+      <c r="F52" s="59">
+        <v>3.5070000000000001</v>
+      </c>
       <c r="G52" s="115"/>
       <c r="H52" s="59" t="s">
         <v>113</v>

</xml_diff>